<commit_message>
Service for Schedule Report
</commit_message>
<xml_diff>
--- a/CTROReporting/CTROReporting/Templates/PDA Abstractor and QC Template.xlsx
+++ b/CTROReporting/CTROReporting/Templates/PDA Abstractor and QC Template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panr2\Downloads\C#\Attitude Loose\Attitude Loose\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panr2\Downloads\C#\CTROReporting\CTROReporting\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{518E053F-13E0-4FBF-9F59-2A3B31592C2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orlando Adan" sheetId="7" r:id="rId1"/>
     <sheet name="Elena Gebeniene" sheetId="8" r:id="rId2"/>
     <sheet name="Temisan Otubu" sheetId="9" r:id="rId3"/>
-    <sheet name="Jamie Phontharaksa" sheetId="10" r:id="rId4"/>
+    <sheet name="Chessie Jones jonesc" sheetId="10" r:id="rId4"/>
     <sheet name="Renae Brunetto brunettor" sheetId="11" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
@@ -478,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -847,85 +848,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1423" displayName="Table1423" ref="A1:H3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
-  <autoFilter ref="A1:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1423" displayName="Table1423" ref="A1:H3" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="58"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="57"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="56"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="55"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="54"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="53"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="52"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Trial ID" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Submission Type" dataDxfId="57"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Submission Number" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Abstractor" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Abstraction Date" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="QC Date" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Abstraction Comments" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="QC Comments" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14234" displayName="Table14234" ref="A1:H3" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
-  <autoFilter ref="A1:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table14234" displayName="Table14234" ref="A1:H3" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="46"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="45"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="44"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="43"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="42"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="41"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="40"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Trial ID" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Submission Type" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Submission Number" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Abstractor" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Abstraction Date" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="QC Date" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Abstraction Comments" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="QC Comments" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table14235" displayName="Table14235" ref="A1:H3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
-  <autoFilter ref="A1:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14235" displayName="Table14235" ref="A1:H3" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="34"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="33"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="32"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="31"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="30"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="29"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="28"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Trial ID" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Submission Type" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Submission Number" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Abstractor" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Abstraction Date" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="QC Date" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Abstraction Comments" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="QC Comments" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table14236" displayName="Table14236" ref="A1:H3" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table14236" displayName="Table14236" ref="A1:H3" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="22"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="21"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="20"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="19"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="18"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="17"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="16"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Trial ID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Submission Type" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Submission Number" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Abstractor" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Abstraction Date" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="QC Date" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Abstraction Comments" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="QC Comments" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table142362" displayName="Table142362" ref="A1:H3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:H3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table142362" displayName="Table142362" ref="A1:H3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:H3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Trial ID" dataDxfId="10"/>
-    <tableColumn id="2" name="Submission Type" dataDxfId="9"/>
-    <tableColumn id="7" name="Submission Number" dataDxfId="8"/>
-    <tableColumn id="3" name="Abstractor" dataDxfId="7"/>
-    <tableColumn id="4" name="Abstraction Date" dataDxfId="6"/>
-    <tableColumn id="8" name="QC Date" dataDxfId="5"/>
-    <tableColumn id="5" name="Abstraction Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="QC Comments" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Trial ID" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Submission Type" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Submission Number" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Abstractor" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Abstraction Date" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="QC Date" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Abstraction Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="QC Comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1227,7 +1228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2003,7 +2004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2779,11 +2780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3555,11 +3556,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="A2:H3"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4331,10 +4332,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -4406,7 +4407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M1977"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>